<commit_message>
Ben bezig met beginopnieuw
</commit_message>
<xml_diff>
--- a/PLSstatic/PLSstatic_predicted_factors_matrix_10.xlsx
+++ b/PLSstatic/PLSstatic_predicted_factors_matrix_10.xlsx
@@ -443,18 +443,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.481909168789137</v>
+        <v>-1.481909168789134</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.274213771939216</v>
+        <v>-4.230807130045484</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.4649429187685064</v>
+        <v>-0.4649429187685051</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.6043943138462237</v>
+        <v>0.7649353906709653</v>
       </c>
     </row>
     <row r="4">
@@ -462,31 +462,31 @@
         <v>1.001341533350507</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8719693715793628</v>
+        <v>-3.18222582427557</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.7242133972617248</v>
+        <v>0.7242133972617233</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6977907676633143</v>
+        <v>0.5215895993778858</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.819227264931658</v>
+        <v>-0.8192272649316585</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.719352489302815</v>
+        <v>-1.970377164371514</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.0938566001430176</v>
+        <v>-0.09385660014301761</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.01089315332504501</v>
+        <v>-0.9361813794003838</v>
       </c>
     </row>
     <row r="8">
@@ -494,31 +494,31 @@
         <v>0.7873815802635769</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6818369935687274</v>
+        <v>0.5227215113784796</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.3310252182837968</v>
+        <v>0.3310252182837974</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3570604735002531</v>
+        <v>0.7865897687033396</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.1876020222794529</v>
+        <v>-0.1876020222794525</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.06290576438928354</v>
+        <v>-2.036259574405221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.2927036682248871</v>
+        <v>0.2927036682248865</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1493013933341931</v>
+        <v>-0.4420696700903583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>